<commit_message>
add function scroll page
</commit_message>
<xml_diff>
--- a/target/classes/BookSelenium.xlsx
+++ b/target/classes/BookSelenium.xlsx
@@ -130,10 +130,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>